<commit_message>
add assertion utils,extent report enhancement
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Login.xlsx
+++ b/src/test/resources/testdata/Login.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>scenerioId</t>
   </si>
@@ -40,6 +40,9 @@
     <t>login twice with IT user</t>
   </si>
   <si>
+    <t>already hit</t>
+  </si>
+  <si>
     <t>shrey.it</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>login with Dr user</t>
   </si>
   <si>
+    <t>success</t>
+  </si>
+  <si>
     <t>shrey.dc</t>
   </si>
   <si>
@@ -67,10 +73,10 @@
     <t>login without username</t>
   </si>
   <si>
+    <t>bad credentials</t>
+  </si>
+  <si>
     <t>NO_DATA</t>
-  </si>
-  <si>
-    <t>Clove@124</t>
   </si>
 </sst>
 </file>
@@ -78,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -92,45 +98,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,14 +175,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -201,22 +208,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,187 +251,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +456,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,47 +542,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -550,40 +562,34 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -592,97 +598,97 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1012,7 +1018,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1055,62 +1061,74 @@
       <c r="C2">
         <v>208</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>200</v>
       </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>400</v>
       </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>